<commit_message>
add db function and review performance from user
</commit_message>
<xml_diff>
--- a/受試者名單.xlsx
+++ b/受試者名單.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\changcheng\Google drive\dp_for_cct\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="13575" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
   <si>
     <t>Timestamp</t>
   </si>
@@ -175,6 +180,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t/>
     </r>
@@ -196,6 +202,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t/>
     </r>
@@ -217,6 +224,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t/>
     </r>
@@ -238,6 +246,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t/>
     </r>
@@ -259,6 +268,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t/>
     </r>
@@ -280,6 +290,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t/>
     </r>
@@ -301,6 +312,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t/>
     </r>
@@ -322,6 +334,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t/>
     </r>
@@ -343,6 +356,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t/>
     </r>
@@ -392,6 +406,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="新細明體"/>
+        <family val="1"/>
         <charset val="136"/>
       </rPr>
       <t>晚上</t>
@@ -408,6 +423,182 @@
   </si>
   <si>
     <t>服科碩二</t>
+  </si>
+  <si>
+    <t>5/14/2014 15:16:55</t>
+  </si>
+  <si>
+    <t>郭明諭</t>
+  </si>
+  <si>
+    <t>工工所</t>
+  </si>
+  <si>
+    <t>5/14/2014 15:27:43</t>
+  </si>
+  <si>
+    <t>碩二</t>
+  </si>
+  <si>
+    <t>5/14/2014 16:57:23</t>
+  </si>
+  <si>
+    <t>5/14/2014 21:13:06</t>
+  </si>
+  <si>
+    <t>王亭茹</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5/23 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>早上</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>kk03232003@gmail.com</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5/27 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>下午</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>m123i456@yahoo.com.tw</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5/28 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>晚上</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>a351397@gmail.com</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>張奕傑</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5/21 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>晚上</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>妤寧</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>高</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>lan88836@gmail.com</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -415,9 +606,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss;@"/>
+    <numFmt numFmtId="176" formatCode="m/d/yyyy\ h:mm:ss;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -438,6 +629,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
     </font>
     <font>
@@ -450,10 +642,37 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,8 +745,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -535,11 +766,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -549,16 +796,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -567,37 +814,37 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -612,12 +859,66 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -943,16 +1244,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="8" max="8" width="54.5" customWidth="1"/>
+    <col min="8" max="8" width="54.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12.75" customHeight="1">
@@ -1329,7 +1630,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="18" customFormat="1" ht="12.75" customHeight="1">
+    <row r="16" spans="1:8" s="18" customFormat="1" ht="12.75" customHeight="1" thickBot="1">
       <c r="A16" s="18">
         <v>15</v>
       </c>
@@ -1355,8 +1656,120 @@
         <v>52</v>
       </c>
     </row>
+    <row r="17" spans="1:8" s="29" customFormat="1" ht="12.75" customHeight="1" thickBot="1">
+      <c r="A17" s="29">
+        <v>16</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="30">
+        <v>912927670</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="33" customFormat="1" ht="12.75" customHeight="1" thickBot="1">
+      <c r="A18" s="33">
+        <v>17</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="34">
+        <v>921525201</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="24">
+        <v>960576200</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
+      <c r="A20" s="18">
+        <v>19</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="26">
+        <v>911961500</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D20" r:id="rId1"/>
+    <hyperlink ref="D17" r:id="rId2"/>
+    <hyperlink ref="D18" r:id="rId3"/>
+    <hyperlink ref="D19" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>